<commit_message>
Chart and documentation updates.
</commit_message>
<xml_diff>
--- a/03_Charts/VAE/XGBoost/BaseModel/Error_Summary.xlsx
+++ b/03_Charts/VAE/XGBoost/BaseModel/Error_Summary.xlsx
@@ -32,7 +32,7 @@
     <t xml:space="preserve">Median_Profit Carried Forward</t>
   </si>
   <si>
-    <t xml:space="preserve">Median_Current Assets</t>
+    <t xml:space="preserve">Median_Liabilities</t>
   </si>
   <si>
     <t xml:space="preserve">True Negative</t>
@@ -404,22 +404,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>130470</v>
+        <v>124608</v>
       </c>
       <c r="C2" t="n">
-        <v>0.248778279521516</v>
+        <v>0.269482442362897</v>
       </c>
       <c r="D2" t="n">
-        <v>0.229853954375418</v>
+        <v>0.248838880007541</v>
       </c>
       <c r="E2" t="n">
-        <v>0.218812975583006</v>
+        <v>0.249657076114419</v>
       </c>
       <c r="F2" t="n">
-        <v>0.215519467897157</v>
+        <v>0.230540219060229</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0317028018751653</v>
+        <v>-0.0500788728053914</v>
       </c>
     </row>
     <row r="3">
@@ -427,22 +427,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>38718</v>
+        <v>44580</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.947440897122465</v>
+        <v>-0.843690993736956</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.970259392941282</v>
+        <v>-0.83887828567755</v>
       </c>
       <c r="E3" t="n">
         <v>-0.624553550835157</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.864505981910226</v>
+        <v>-0.760497939050802</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.123519379739956</v>
+        <v>0.103074222886388</v>
       </c>
     </row>
     <row r="4">
@@ -450,22 +450,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>312</v>
+        <v>175</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0177958937019884</v>
+        <v>0.0104436174992944</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.041609502958233</v>
+        <v>-0.0400732388617184</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.0783617661165398</v>
+        <v>0.0774335872267252</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0623410579204389</v>
+        <v>0.0290282858566791</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.0799162879830036</v>
+        <v>0.0214540030466988</v>
       </c>
     </row>
     <row r="5">
@@ -473,22 +473,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>1154</v>
+        <v>1291</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.09896382918476</v>
+        <v>-0.991959669159165</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.08217885192642</v>
+        <v>-1.00821067376228</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.624553550835157</v>
+        <v>-0.567911524566636</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.891749699930934</v>
+        <v>-0.800272521643408</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.0576470527434416</v>
+        <v>0.162951274448651</v>
       </c>
     </row>
   </sheetData>

</xml_diff>